<commit_message>
feat: sub type 로직 적용
</commit_message>
<xml_diff>
--- a/public/newquestion-data.xlsx
+++ b/public/newquestion-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Root\Desktop\test\SEAL-project\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAF7622-85E0-4B57-A69C-4B0783FA8E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35013D3-F2FC-453B-B323-049578FAA212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="601" activeTab="2" xr2:uid="{3CEA7212-19CA-44FB-9704-8721F14797E9}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="601" firstSheet="1" activeTab="3" xr2:uid="{3CEA7212-19CA-44FB-9704-8721F14797E9}"/>
   </bookViews>
   <sheets>
     <sheet name="절대문항-main" sheetId="1" r:id="rId1"/>
@@ -39,16 +39,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="210">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>weight</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>value</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -158,10 +154,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>null</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RELM02</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -187,18 +179,6 @@
   </si>
   <si>
     <t>M011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>answer1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>answer2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>answer3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -402,34 +382,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>상황 1: 팀 프로젝트 중 의견 차이로 인해 격한 논쟁이 벌어졌다.</t>
-  </si>
-  <si>
-    <t>상황 2: 팀원이 개인적인 문제로 인해 업무에 집중하지 못하고 있다.</t>
-  </si>
-  <si>
-    <t>상황 3: 새로운 팀원이 업무 환경에 적응하는 데 어려움을 겪고 있다.</t>
-  </si>
-  <si>
-    <t>상황 4: 프로젝트 진행 중 예상치 못한 문제점이 발생했다.</t>
-  </si>
-  <si>
-    <t>상황 5: 새로운 작업 절차를 도입해야 한다.</t>
-  </si>
-  <si>
-    <t>상황 6: 프로젝트 목표를 달성하기 위해 팀을 이끌어야 한다.</t>
-  </si>
-  <si>
-    <t>상황 7: 기존의 방식을 개선하거나 새로운 아이디어를 도입해야 한다.</t>
-  </si>
-  <si>
-    <t>상황 8: 팀 프로젝트 중 의견 차이로 인해 격한 논쟁이 벌어졌다.</t>
-  </si>
-  <si>
-    <t>촉진자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>S011</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -530,14 +482,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>조정자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조언자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>tier</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -717,6 +661,118 @@
   <si>
     <t>priority</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회사 내에서 갈등이 발생했을 때, 당신의 반응은?</t>
+  </si>
+  <si>
+    <t>양측 모두의 입장을 들어보고, 이해하려고 한다</t>
+  </si>
+  <si>
+    <t>갈등을 해결하기 위한 방법을 생각해본다</t>
+  </si>
+  <si>
+    <t>상황을 진정시키고, 갈등이 커지지 않을 방법을 찾는다</t>
+  </si>
+  <si>
+    <t>업무 마감일이 다가오지만 팀원이 작업을 완료하지 못했을 때, 당신의 반응은?</t>
+  </si>
+  <si>
+    <t>무엇이 어려운지 묻고, 일을 잘 할수 있도록 조언을 제공한다</t>
+  </si>
+  <si>
+    <t>문제의 원인을 파악하여, 해결 방안을 제시한다</t>
+  </si>
+  <si>
+    <t>팀 회의 중 새로운 아이디어가 필요할 때, 당신의 반응은?</t>
+  </si>
+  <si>
+    <t>기존의 방식에서 떠난 새로운 접근으로 아이디어를 제시해본다</t>
+  </si>
+  <si>
+    <t>최신 정보를 바탕으로 아이디어를 구상하여 제시한다</t>
+  </si>
+  <si>
+    <t>팀원들이 자유로운 이야기 속에서 아이디어를 낼 수 있게 분위기를 조성한다</t>
+  </si>
+  <si>
+    <t>데이터 분석 결과가 예상과 다를 때, 당신의 반응은?</t>
+  </si>
+  <si>
+    <t>계획을 전체적으로 재검토하고, 새로운 계획을 세우려고 한다</t>
+  </si>
+  <si>
+    <t>결과를 분석하여, 어느 부분이 예상에서 벗어나게 된 원인인지 파악한다</t>
+  </si>
+  <si>
+    <t>이 분석을 바탕으로 장기적인 미래에 대해 검토해본다</t>
+  </si>
+  <si>
+    <t>새로운 기술을 도입해야 할 때, 당신의 반응은?</t>
+  </si>
+  <si>
+    <t>우선 새로운 기술을 학습해보고, 학습 내용을 팀에 공유한다</t>
+  </si>
+  <si>
+    <t>새로운 기술이 미래에 미칠 영향을 알아본다</t>
+  </si>
+  <si>
+    <t>도입하기 전에, 기존의 기술과 함께 사용해도 괜찮은지 확인해본다</t>
+  </si>
+  <si>
+    <t>갑자기 발생한 문제, 신속한 결정을 내려야 할 떄, 당신의 반응은?</t>
+  </si>
+  <si>
+    <t>직감에 따라서 빠르게 결정한다</t>
+  </si>
+  <si>
+    <t>신속하게 실행시킬 수 있는 방법으로 대응한다</t>
+  </si>
+  <si>
+    <t>팀원들의 의견을 수렴하여 결정을 내린다</t>
+  </si>
+  <si>
+    <t>업무 성과가 기대에 미치지 못할때, 당신의 반응은?</t>
+  </si>
+  <si>
+    <t>팀원들과 업무 성과에 개선 방향에 대해 논의해본다</t>
+  </si>
+  <si>
+    <t>성과를 개선할 새로운 아이디어를 생각해본다</t>
+  </si>
+  <si>
+    <t>업무 목표치를 보면서, 장기적인 성공을 위한 계획을 다시 세운다</t>
+  </si>
+  <si>
+    <t>갑작스럽게 직무가 변경되었을 때, 당신의 반응은?</t>
+  </si>
+  <si>
+    <t>직무 변경을 기회로 삼아, 새로운 업무에 적극적으로 임한다</t>
+  </si>
+  <si>
+    <t>새 직무의 요구사항을 이해하고, 능력을 발휘할 수 있는 방법을 찾아본다</t>
+  </si>
+  <si>
+    <t>새 직무에 맞춰 나의 목표를 다시 계획한다</t>
+  </si>
+  <si>
+    <t>남은 시간을 고려하여 팀원의 작업량을 조정해준다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설계자</t>
+  </si>
+  <si>
+    <t>상담가</t>
+  </si>
+  <si>
+    <t>발명가</t>
+  </si>
+  <si>
+    <t>학자</t>
+  </si>
+  <si>
+    <t>비전가</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1178,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1135,30 +1191,30 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="F1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1172,13 +1228,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1192,13 +1248,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1212,13 +1268,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1232,13 +1288,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1252,13 +1308,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1272,13 +1328,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1292,13 +1348,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1312,13 +1368,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1332,13 +1388,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1352,13 +1408,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1372,13 +1428,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1401,7 +1457,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E13"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1415,220 +1471,220 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1641,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748C9573-87FC-4119-B4BA-FD8432D5A901}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1656,27 +1712,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -1684,13 +1740,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1704,13 +1760,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1724,13 +1780,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -1744,13 +1800,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1764,10 +1820,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -1775,13 +1831,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1795,13 +1851,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1815,13 +1871,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1835,13 +1891,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -1855,10 +1911,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -1866,13 +1922,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -1886,13 +1942,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -1906,13 +1962,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1926,13 +1982,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1946,10 +2002,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -1957,13 +2013,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1977,13 +2033,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -1997,13 +2053,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -2017,13 +2073,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -2037,10 +2093,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -2048,13 +2104,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -2068,13 +2124,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -2088,13 +2144,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -2108,13 +2164,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="B26" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2128,10 +2184,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -2139,13 +2195,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -2159,13 +2215,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -2179,13 +2235,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -2199,13 +2255,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="B31" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31">
         <v>4</v>
@@ -2219,10 +2275,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -2230,13 +2286,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -2250,13 +2306,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -2270,13 +2326,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -2290,13 +2346,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B36" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -2321,576 +2377,603 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC3D32F-513C-447A-949B-8A0B51E190FD}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="60.75" customWidth="1"/>
+    <col min="2" max="2" width="68.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="D1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" t="s">
+        <v>209</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>188</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>88</v>
       </c>
-      <c r="B2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B22" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>106</v>
       </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B23" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>107</v>
       </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>89</v>
       </c>
-      <c r="B6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>109</v>
       </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B27" t="s">
+        <v>197</v>
+      </c>
+      <c r="C27" t="s">
+        <v>206</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>110</v>
       </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C28" t="s">
+        <v>207</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" t="s">
+        <v>199</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>90</v>
       </c>
-      <c r="B10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B30" t="s">
+        <v>200</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>112</v>
       </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B31" t="s">
+        <v>201</v>
+      </c>
+      <c r="C31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>113</v>
       </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B32" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>114</v>
       </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>131</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>117</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>118</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>120</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" t="s">
-        <v>130</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>122</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>123</v>
-      </c>
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>127</v>
-      </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>128</v>
-      </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>203</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" t="s">
-        <v>131</v>
+        <v>81</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: resultpage max 값 수정
</commit_message>
<xml_diff>
--- a/public/newquestion-data.xlsx
+++ b/public/newquestion-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Root\Desktop\SEAL-project\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8E17A5-EBD4-48A0-A0D0-85F0A28F27E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D49B337-7BB2-45DA-9561-588AFF4CF965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="601" firstSheet="1" activeTab="3" xr2:uid="{3CEA7212-19CA-44FB-9704-8721F14797E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" tabRatio="601" firstSheet="1" activeTab="3" xr2:uid="{3CEA7212-19CA-44FB-9704-8721F14797E9}"/>
   </bookViews>
   <sheets>
     <sheet name="절대문항-main" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="215">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -252,27 +252,15 @@
     <t>팀 회의 중 동료가 새로운 아이디어를 제시했습니다. 어떻게 반응하십니까?</t>
   </si>
   <si>
-    <t>좋은 아이디어인 것 같은데, 함께 발전시킬 방법이 있을지 생각해본다</t>
-  </si>
-  <si>
     <t>이와 비슷한 다른 아이디어들도 제안하면서 논의한다</t>
   </si>
   <si>
-    <t>아직 확실하진 않으니, 지금의 전략을 유지하는 것이 좋을 것 같다</t>
-  </si>
-  <si>
     <t>아이디어에 대한 근거나 자료가 있는지, 동료에게 요청한다</t>
   </si>
   <si>
-    <t>팀의 업무 수행 계획에 예상치 못한 변화가 생겼습니다. 어떻게 대처하십니까?</t>
-  </si>
-  <si>
     <t>팀원들과 협력하여, 변화에 대한 해결책을 찾아본다</t>
   </si>
   <si>
-    <t>변화를 기회로 삼아 빠르게 대응하는 것에 집중한다</t>
-  </si>
-  <si>
     <t>최대한 기존 계획을 유지할 수 있도록 변화에 대처한다</t>
   </si>
   <si>
@@ -282,9 +270,6 @@
     <t>팀 내 갈등 상황이 발생했습니다. 어떻게 해결하십니까?</t>
   </si>
   <si>
-    <t>양 쪽의 입장을 듣고, 서로 원만하게 해결할 수 있도록 중재한다</t>
-  </si>
-  <si>
     <t>갈등이 오래 지속되지 않도록 신속하게 조치를 취한다</t>
   </si>
   <si>
@@ -318,9 +303,6 @@
     <t>도입 전에 프로세스를 먼저 시험해보고, 문제가 있는지 확인해본다</t>
   </si>
   <si>
-    <t>기존의 업무 프로세스와 비슷한 형태로 진행할 수 있는지 확인해본다</t>
-  </si>
-  <si>
     <t>새로운 업무 프로세스에 대한 정보부터 확인한다</t>
   </si>
   <si>
@@ -348,15 +330,9 @@
     <t>팀 회의 중 새로운 아이디어가 필요할 때, 당신의 반응은?</t>
   </si>
   <si>
-    <t>기존의 방식에서 떠난 새로운 접근으로 아이디어를 제시해본다</t>
-  </si>
-  <si>
     <t>최신 정보를 바탕으로 아이디어를 구상하여 제시한다</t>
   </si>
   <si>
-    <t>팀원들이 자유로운 이야기 속에서 아이디어를 낼 수 있게 분위기를 조성한다</t>
-  </si>
-  <si>
     <t>데이터 분석 결과가 예상과 다를 때, 당신의 반응은?</t>
   </si>
   <si>
@@ -708,20 +684,1088 @@
     <t>S082</t>
   </si>
   <si>
-    <t>팀원들과의 교류를 통해 새 직무에 적응하는데 필요한 경험이나 정보를 물어본다</t>
-  </si>
-  <si>
     <t>S083</t>
   </si>
   <si>
     <t>새로운 직무에 잘 적응하기 위한 계획을 세워본다</t>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>괜찮은 아이디어라면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>함께</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>발전시킬</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>방법을 고려해본다</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아직</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>확실하진</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>않으니</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지금의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전략을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>유지하는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>것이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>좋을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>것</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>같다</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>팀</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>업무</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>계획에</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>예상치</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>못한</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>변화가</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>생겼습니다</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>어떻게</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>대처하십니까</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>변화를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기회로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삼아</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>빠르게</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>대응하는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>것에 집중한다</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>양</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>쪽의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>입장을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">모두 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>듣고</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>원만하게</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해결할</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있도록</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>중재한다</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기존</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>업무</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로세스와</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>비슷한</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>형태로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>진행할</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있는지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>확인해본다</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기존</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>방식에서</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>벗어난</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>새로운</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>접근으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아이디어를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>제시해본다</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀원들이 다양한 아이디어를 낼 수 있도록 편안한 분위기를 조성한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="새굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>직무</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>에 적응하기 위해 필요한 경험이나 정보를 팀원들에게 물어본다</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,6 +1799,65 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="새굴림"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="새굴림"/>
+      <family val="1"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="1"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="새굴림"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="새굴림"/>
+      <family val="1"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="돋움"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -794,7 +1897,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -812,6 +1915,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1463,7 +2578,7 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1477,10 +2592,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1497,7 +2612,7 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1514,7 +2629,7 @@
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1528,10 +2643,10 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1545,10 +2660,10 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1565,7 +2680,7 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1579,10 +2694,10 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1596,10 +2711,10 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1616,7 +2731,7 @@
         <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1633,7 +2748,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1650,7 +2765,7 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1670,7 +2785,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1681,27 +2796,27 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>53</v>
@@ -1715,13 +2830,13 @@
     </row>
     <row r="3" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -1735,13 +2850,13 @@
     </row>
     <row r="4" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -1755,13 +2870,13 @@
     </row>
     <row r="5" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D5" s="4">
         <v>4</v>
@@ -1775,13 +2890,13 @@
     </row>
     <row r="6" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -1795,7 +2910,7 @@
     </row>
     <row r="7" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>58</v>
@@ -1809,13 +2924,13 @@
     </row>
     <row r="8" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>134</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>206</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D8" s="4">
         <v>2</v>
@@ -1829,13 +2944,13 @@
     </row>
     <row r="9" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -1849,13 +2964,13 @@
     </row>
     <row r="10" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>136</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>207</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D10" s="4">
         <v>3</v>
@@ -1869,13 +2984,13 @@
     </row>
     <row r="11" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D11" s="4">
         <v>4</v>
@@ -1889,10 +3004,10 @@
     </row>
     <row r="12" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>63</v>
+        <v>138</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>208</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1903,13 +3018,13 @@
     </row>
     <row r="13" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D13" s="4">
         <v>3</v>
@@ -1923,13 +3038,13 @@
     </row>
     <row r="14" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>140</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>209</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D14" s="4">
         <v>4</v>
@@ -1943,13 +3058,13 @@
     </row>
     <row r="15" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D15" s="4">
         <v>2</v>
@@ -1963,13 +3078,13 @@
     </row>
     <row r="16" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -1983,10 +3098,10 @@
     </row>
     <row r="17" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1997,13 +3112,13 @@
     </row>
     <row r="18" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>144</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -2017,13 +3132,13 @@
     </row>
     <row r="19" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D19" s="4">
         <v>3</v>
@@ -2037,13 +3152,13 @@
     </row>
     <row r="20" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D20" s="4">
         <v>2</v>
@@ -2057,13 +3172,13 @@
     </row>
     <row r="21" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D21" s="4">
         <v>4</v>
@@ -2077,10 +3192,10 @@
     </row>
     <row r="22" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2091,13 +3206,13 @@
     </row>
     <row r="23" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D23" s="4">
         <v>3</v>
@@ -2111,13 +3226,13 @@
     </row>
     <row r="24" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D24" s="4">
         <v>4</v>
@@ -2131,13 +3246,13 @@
     </row>
     <row r="25" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D25" s="4">
         <v>2</v>
@@ -2151,13 +3266,13 @@
     </row>
     <row r="26" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
@@ -2171,10 +3286,10 @@
     </row>
     <row r="27" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2185,13 +3300,13 @@
     </row>
     <row r="28" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D28" s="4">
         <v>3</v>
@@ -2205,13 +3320,13 @@
     </row>
     <row r="29" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
@@ -2225,13 +3340,13 @@
     </row>
     <row r="30" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D30" s="4">
         <v>2</v>
@@ -2245,13 +3360,13 @@
     </row>
     <row r="31" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D31" s="4">
         <v>4</v>
@@ -2265,10 +3380,10 @@
     </row>
     <row r="32" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -2279,13 +3394,13 @@
     </row>
     <row r="33" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D33" s="4">
         <v>4</v>
@@ -2299,13 +3414,13 @@
     </row>
     <row r="34" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
@@ -2319,13 +3434,13 @@
     </row>
     <row r="35" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>166</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D35" s="4">
         <v>3</v>
@@ -2339,13 +3454,13 @@
     </row>
     <row r="36" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D36" s="4">
         <v>2</v>
@@ -2365,10 +3480,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC3D32F-513C-447A-949B-8A0B51E190FD}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2376,32 +3491,32 @@
     <col min="2" max="2" width="68.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2410,12 +3525,12 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>34</v>
@@ -2430,12 +3545,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>35</v>
@@ -2450,12 +3565,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -2470,12 +3585,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2484,15 +3599,15 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -2504,15 +3619,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D8" s="4">
         <v>2</v>
@@ -2524,12 +3639,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>37</v>
@@ -2544,12 +3659,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -2558,15 +3673,15 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>178</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>212</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -2578,15 +3693,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D12" s="4">
         <v>2</v>
@@ -2598,12 +3713,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>93</v>
+        <v>180</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>213</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>31</v>
@@ -2618,12 +3733,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -2631,16 +3746,19 @@
         <v>3</v>
       </c>
       <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -2652,12 +3770,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>37</v>
@@ -2674,13 +3792,13 @@
     </row>
     <row r="17" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D17" s="4">
         <v>3</v>
@@ -2694,10 +3812,10 @@
     </row>
     <row r="18" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2708,13 +3826,13 @@
     </row>
     <row r="19" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D19" s="4">
         <v>3</v>
@@ -2728,13 +3846,13 @@
     </row>
     <row r="20" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D20" s="4">
         <v>2</v>
@@ -2748,10 +3866,10 @@
     </row>
     <row r="21" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>35</v>
@@ -2768,10 +3886,10 @@
     </row>
     <row r="22" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2782,10 +3900,10 @@
     </row>
     <row r="23" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2802,10 +3920,10 @@
     </row>
     <row r="24" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>33</v>
@@ -2822,10 +3940,10 @@
     </row>
     <row r="25" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>31</v>
@@ -2842,10 +3960,10 @@
     </row>
     <row r="26" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2856,13 +3974,13 @@
     </row>
     <row r="27" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D27" s="4">
         <v>3</v>
@@ -2876,13 +3994,13 @@
     </row>
     <row r="28" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D28" s="4">
         <v>2</v>
@@ -2896,10 +4014,10 @@
     </row>
     <row r="29" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>36</v>
@@ -2916,10 +4034,10 @@
     </row>
     <row r="30" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2930,10 +4048,10 @@
     </row>
     <row r="31" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -2950,10 +4068,10 @@
     </row>
     <row r="32" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>214</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>34</v>
@@ -2970,10 +4088,10 @@
     </row>
     <row r="33" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>36</v>

</xml_diff>